<commit_message>
Get daily reddit data: Tue Jun 17 08:13:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_22.xlsx
+++ b/data/collected_data/2025_06_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C503"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3440 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ldgqkt</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Neon 80s Summer nail.</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldgqkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ldggf1</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>My new colorful 3d flower nails🥰🌸</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldggf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ldg5nl</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>girl is going to Amalfi with this set🍊🫐🍒</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xleo6y0nf7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ldfyq2</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Primark press on nails.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0e25putkf7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ldfaxk</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Summerween nails 💅</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8av72yaadf7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ld6slx</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>How do I fix the whites of my nails?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ld6slx/how_do_i_fix_the_whites_of_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ldcxsw</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Help?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldcxsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ldevtj</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Will press ons last longer than gel for brittle nails?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ldevtj/will_press_ons_last_longer_than_gel_for_brittle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ldevrg</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>First time making junk nails, How’d I do?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldevrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ldeqra</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>I hope you like this glaze I made</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3esgn7m57f7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ldediw</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>A nude moment 🎀</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldediw</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1lddm8m</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>How badly did I mess up my nails?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pkjq1iive7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1ldbfzw</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Help a girl out pls 😊</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/582ss02nbe7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ldbmcz</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Should I get these redone?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldbmcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ldct1j</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Avril Lavigne inspired after attending her concert. I think she'd be proud</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldct1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1ldc536</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Birthday set ✨</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceteggmuhe7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1lddct5</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Apple nails</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqqbghzyse7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ldd8d5</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>gel on my natural nails, i’m enjoying the fun designs lately</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldd8d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ldckc3</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Just got these today!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldckc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ldci9w</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>did my nails for vacation!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fbr7pf7le7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ldcg4b</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>i’m 21 and i just hit a year of not biting my nails :))</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tetd4upoke7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ldc90l</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Bi flag?✅ Holo glitter?✅ Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/150crihuie7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ldbehc</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>My girl is amazing 😍</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rbx26fa9be7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ldbb16</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>I’m taken aback by how beautiful these are</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldbb16</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ld9bja</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>the picture vs the execution</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld9bja</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ldajq3</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Do i get these fixed?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldajq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1lda8nd</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>So, where do I go from here?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lda8nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ldam8o</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>POOLSIDE ALL SUMMER PLZ</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldam8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ldafkq</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Help/ Advice for First Manicure?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldafkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1lda9zx</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>They're not great but they are an experiment</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65lxyzvr0e7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1lda8hc</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Cracked nails</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lda8hc/cracked_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ld99sx</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>First dip</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld99sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ld98d3</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Cute or nah?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32tlxpp5sd7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ld95ck</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Nails for Pride Month! 🏳️‍🌈🏳️‍🌈🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpp4lw4grd7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ld93ub</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Those with cool skin tones: any favourite nail polish colours??</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ld93ub/those_with_cool_skin_tones_any_favourite_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ld8szh</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>I got my nails done with my girlfriend for the first time .</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld8szh</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ld8b0c</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>🍨🍦summer is here!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rysp4s93kd7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ld7eb4</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>at home moo nails 🐄🐮</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdfzhvq3dd7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ld7c28</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>new pink set</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vdnlp7yocd7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ld6iba</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Proud of this set!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld6iba</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ld69b5</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Can someone tell me that the nails I got are cute bc l'm actually crying in the parking lot rn (third photo was my reference I gave her)</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld69b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ld685a</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz6ogkl94d7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ld48jd</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Addition to my last post</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jer964k3qc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ld4oil</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>how do you get acrylic to stick?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ld4oil/how_do_you_get_acrylic_to_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ld4x7u</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Happy pride!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld4x7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ld4hgf</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Pride Nails!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66vsnditrc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ld4gcx</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>my new blue set</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3iff7olrc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ld4f2c</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Birthday Set</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld4f2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ld45ay</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Goodbye gems</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld45ay</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ld407x</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Seashells</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mapayltgoc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ld3xbk</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Custom summer press on set! 🌸🫧</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld3xbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ld2zm6</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>SOS need advice, what can I do to fix them?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld2zm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ld2tss</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>What shape?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgpi22qdgc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ld26df</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>I injured my nail bed with acrylics on and now it is torn. How do I move forward?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld26df</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ld2dw5</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Forest fairy nails!</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld2dw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ld24ak</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>The press-ons I had for my brothers wedding!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld24ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ld1269</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Real nail lifted with gel X extension, won't stop oozing liquid -</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld1269</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ld0t1g</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Are these as bad as I think?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld0t1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ld1rq7</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>new new</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juyf8asz8c7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ld1kzw</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Cherry picnic nails- approved by 1 out of 2 dogs</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld1kzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ld1j4b</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>First time poster…</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tshuk7wc7c7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ld19hx</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Santa Muerte set I did!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld19hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ld12io</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Not sure how I feel about my French tip nails?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld12io</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ld11qh</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>advice on how to keep nails healthy and long, as a long term nail biter</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld11qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ld0o83</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Swedish midsummer nails!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujkuxidj1c7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ld0e5p</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>First shellac mani/pedi</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ld0e5p/first_shellac_manipedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1lczeyn</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Took me all day</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lczeyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1lczc54</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Went for earthy, came out Dubai chocolate 🤦🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79r50w4vsb7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1lcz1o6</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Mercedes won in F1 Canadian GP, so…….</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dmhlygzqb7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1lcyywl</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>New to this, need some help please!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o0w448gqb7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1lcynqp</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Watermelon</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1iat8ceob7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1lcyhlg</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>My first nail art 🪻</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcyhlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1lcyfnv</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Will Luminary’s lamp cure DND gel polishes? And also, which DND gel line is pure gel?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lcyfnv/will_luminarys_lamp_cure_dnd_gel_polishes_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1lcxthj</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Nails turned out terrible - I’m horribly depressed salon wants to charge me again - when it’s only been three days!!!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcxthj</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1lcxm8q</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Is this brand safe to use?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ng844ghhb7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1lcxb9d</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Thoughts???</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcxb9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1lcwtp3</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>how do i fix this? or is there no way</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcwtp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1lculi9</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>caught nail on a hook and it bent ; what's happened?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8spc47jbva7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1lcuwjt</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izcbq5fzya7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1lcqppy</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Nail Thoughts or Kokoist Platinum Filler Base for builder gel?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3ryp8wz1a7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1lcw8b6</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>My Amazing Wedding Nails!</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcw8b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1lcwkn7</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>whats the trick to making cuticles look good</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e264iv7aab7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1lcwd85</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>New week new nails 💅</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxo3b5ez8b7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1lcw593</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Pretty or nah??</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5pzk4gf7b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1lcw16i</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Acrylics keep popping off?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rpo4lto6b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1lcvyye</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Glitter top coat peeling off?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quf47x7a6b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1lcvxln</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Getting back into it!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtdsjpu06b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1lcvwy1</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>First time having nails extension</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhim7w7w5b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1lcvm08</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>🍒Cherry on top🍒</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2bmi14u3b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1lcvi7b</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>I feel prettier than ever with this black set. Love CatEye.</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcvi7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1lcv5en</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Summer Nails!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw17r5ao0b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1lcuzff</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Fairy Wing Nails!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcuzff</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1lcuy33</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9kynmcaza7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1lcuslc</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Pisces nails :)</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8qhtyem4ya7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1lcufjr</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Best rubber base and hard gel product?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lcufjr/best_rubber_base_and_hard_gel_product/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1lcu98b</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>My 16 yr old sister does nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcu98b</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1lcto75</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Lemon cream nails</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lcto75/lemon_cream_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1lctenw</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Pre-polishing gel x nails</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lctenw/prepolishing_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1lctc3f</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Has anyone ever seen this before?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2f7joebna7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1lct6b3</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Kept it simple this time- Thoughts?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qth8vxmmma7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ldgfn0</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Yet another Pride mani</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldgfn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ldg833</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Nail growth tips/advice</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldg833/nail_growth_tipsadvice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ldfb1o</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Pearl for June</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tcptepbdf7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ldesge</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Not A Polish Flex</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldesge</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ldeb4n</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>After 5+ Years!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldeb4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ldcrvr</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Help me find this salon polish brand, please!</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldcrvr/help_me_find_this_salon_polish_brand_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ldchff</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Perfect base to shimmer ratio</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldchff</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ldca1y</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Feeling like an intergalactic ice princess?🌌🤍</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldca1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ldc1v9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers suggestions</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldc1v9/alchemy_lacquers_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ldb6st</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Finally organized the way I want it!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldb6st</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ldarl2</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Dupe requests for ILNP and Mooncat</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldarl2/dupe_requests_for_ilnp_and_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ldamvy</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>🌺petals🌺</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldaknx</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ldakro</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Cotopaxi-inspired mani</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1lee4py3e7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ldagwe</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Little bits of nail on sidewall that always want to separate? Any tips?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldagwe/little_bits_of_nail_on_sidewall_that_always_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1lda7yx</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>phoenix polish “sarah”</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z99ffwpt0e7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1lda43w</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>New Favorite Combo Alert</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4y017ratzd7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ld8mgf</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>I've had this colour forever</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld8mgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ld8hcw</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>My Fancy Gloss arrived!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld8hcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ld84px</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Admiring my (near) perfect white mani before I ruin it with nail art</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ld84px/admiring_my_near_perfect_white_mani_before_i_ruin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ld7x3g</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>i remain, as ever, absolutely obsessed</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9p46ieldhd7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ld7wdk</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Manucurist Paris customer service</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld7wdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ld7p6i</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Sunshiny Day</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld7p6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ld7irc</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Touch up remover jar</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/anbliov6ed7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ld7dma</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Welcome to a new sub for the Southern Hemisphere lacqueristas 🌏 r/SouthHemisphereNails</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej26t4k2dd7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ld767z</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Please help me pick a coral ❤️🧡</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j52sfdbgbd7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ld71z6</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Sunflower Skittle</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld71z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ld6fkk</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Wiener Dog Green</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld6fkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ld63ar</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Swatching Magnetics En Masse</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld63ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ld5dc6</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>There’s no such thing as too much blue 🔵</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld5dc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ld50eu</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>🥭🥭🥭</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld50eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1ld4yxl</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>First time growing my nails and trying polish at home, in love so far!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmdejst5vc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ld42cv</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Fancy Gloss: Ocean Quartz (over black)</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3dgxc9woc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ld3l1e</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Lurid must haves from June restocks</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ld3l1e/lurid_must_haves_from_june_restocks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ld3dcn</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>When you realize at the party your nails are black light reactive so you lock yourself in a toilet to do pics 😂</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld3dcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ld393r</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Whiskey Sunrise</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld393r</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ld2yad</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>BELIEVE BEAUTY SKITTLE</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp76f1n8hc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ld2tsw</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Bragging about my find</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9xfjlpdgc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ld2kmg</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>What is your favorite Aurora powder from Amazon?  I recently got one and it's amazing but for seven bucks you hardly get anything.</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ld2kmg/what_is_your_favorite_aurora_powder_from_amazon_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ld263g</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Well ur time has come my dears 🥲</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld24fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ld0sba</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Swatch request: Curiosity's Prey Dupe as topper</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld0sba</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ld0jg1</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Lurid - On the Prowl</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld0jg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ld0itj</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Am I doing magnetic wrong?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld0itj</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ld0daq</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>100/10 Red Eyed Lacquer Packaging!</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1qjfzghzb7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ld027t</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>The illusions of Illusionist</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lasvo5sfxb7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1lczvdx</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Seche Vite Advice Needed</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/396iesw9wb7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1lczrn8</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>I’m always on the lookout for unique magnetic shifts</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/15x4a0givb7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1lczr2i</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Sunburst</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lczr2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1lcze5m</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Infinite Nebula transition from shade to sun😎</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dvscovq7tb7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1lczadh</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>messy frogs</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lczadh</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1lcv7u5</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>So-Called Salon Nails (DIY Kit)</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcv7u5/socalled_salon_nails_diy_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1lcvucp</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Glitter top coat peeling off?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5atatple5b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1lcyusg</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>a rainbow on every nail 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcyusg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1lcxd9h</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Neon Shimmer Rainbow Skittle</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcxd9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1lcytdp</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>ILNP Amber + Glory</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcytdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1lcxejd</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Looking for a midnight/cobalt blue Essie I had in 2005</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcxejd/looking_for_a_midnightcobalt_blue_essie_i_had_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1lcxbpw</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Am I shifty-nail-polish blind?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kredju7hfb7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1lcxad7</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Pretty in ILNP - Pixel Pink ft. Rogue - Rock &amp; A Hard Place</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w4i26za5fb7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1lcwykh</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Mermaid vibes</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcwykh</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1lcwu6f</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>All aboard the thermals are super fun train!</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcwu6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1lcwtig</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>neptune fantasy 💙</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcwtig</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1lcwoh2</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>If Frogs (Almost) Had Wings</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcwoh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1lcwizi</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Lumen-Magic Frog</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcwizi</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1lcwa4u</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>ILNP On Location</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdhit53d8b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1lcw4a9</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Help with Crooked Nail</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcw4a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1lcvw27</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>La Petite Mort</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yk4atyxp5b7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1lcv4ex</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Best crème rainbow sets for nail art?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcv4ex/best_crème_rainbow_sets_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1lcv3dn</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I love light toned magnetics</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kp877ilcya7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1lcv2bz</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>True Mirror Polish</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcv2bz/true_mirror_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1lcutry</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>As requested: Google doc for Mooncat dupes!</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcutry/as_requested_google_doc_for_mooncat_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1lcumah</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Simple Little Sheer Mani</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcumah</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1lcui7d</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Lyn B Designs fragrance</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcui7d/lyn_b_designs_fragrance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1lcu65p</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Stopping in the middle of the street to catch ILNP Warped in the sun</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/09xr2fajta7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1lcty1r</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>You know her, you love her 👻</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcty1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1lctk45</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>egg egg egg egg 🍳🍳🍳 [gifted PR]</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lctk45</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1lcsud9</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat’s top coat?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcsud9/dupe_for_mooncats_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1lcskhc</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Attempted cute nail pics with my cat… instantly regretted it</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcskhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1lcru4x</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>high fae magic ✨</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8dp5qg1ca7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1lcrtvj</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>am i the only one who prefers a diffused cat eye?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v57csv3zba7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1lcrqbm</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>No uv gel polish recommendations.</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcrqbm/no_uv_gel_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1lcrpbb</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Let me put y’all onto something</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcrpbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1lcqqcf</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>first time getting nails done. gap at the side of my nail?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcqqcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1lcqjhd</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Long time lurker, first time poster! Also a nail noob 🫡</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv824e5cz97f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1lcpzqg</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Didn’t expect this from a £3 magnetic 🧲</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcpzqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1lcow2b</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lcow2b/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1lco05t</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Can you help me identify these Masura shades?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lco05t/can_you_help_me_identify_these_masura_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1ldh6w5</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Practicing</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meemmisgzf7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1ldcvao</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>i need some advice or tips to make the powder stick only to the design🙏🏾🙏🏾 ✨💕i've tried several techniques and still haven't achieved a clean design 🥺😔</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rogtmjgoe7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1ldcokw</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Hoy me tocó ser modelo de uñas de mi mamá 🥰</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b2ms6lsme7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1ld9e1v</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>bears and bows</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld9e1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ld8i7f</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>So I did a thing today 😫💕 any comments</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld8i7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ld5f55</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Circus themed nails!!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9c1s28eyc7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ld2uvs</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I got carried away… and I got a surprise.</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ld2uvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1lczabp</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Random practice nails</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajx5nrijsb7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1lcz3ih</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Hi these are my first finished attempts</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcz3ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1lcyiro</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>My first nail art 🪻</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcyiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1lcxoh0</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Lemon nails~</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcxoh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1lcvxlj</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Glitter top coat peeling off?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tskmaf116b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1lcvcn5</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Summer press on set! 🌸🫧</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1el8fv12b7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1lcusud</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Starry night 💛✨</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jaw5z79ya7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1lcu44a</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>My 16 yr old sisters nail art</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcu44a</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1lcrhc2</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Emo 4eva 🖤🏴‍☠️</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcrhc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1lcogm6</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>monet-inspired water lily nails 🩷🎨</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lcogm6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun 18 08:13:09 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_22.xlsx
+++ b/data/collected_data/2025_06_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C503"/>
+  <dimension ref="A1:C714"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8984,6 +8984,3593 @@
         </is>
       </c>
     </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1lebibb</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Sanrio Kawaii Set</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lebibb</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1lebbnd</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Help! Superglue on new gel manicure!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lebbnd/help_superglue_on_new_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1leb9l2</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Cute nails made by me</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mzzbi5y4n7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1leb1rv</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Homemade: Experimenting with French tip and colors</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxyjfvr82n7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1leazef</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Nails progress 3 weeks</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leazef</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1leako6</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>How’s my pedicure?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05zvmm8nwm7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1leac5k</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>a first for my nail tech i think they did great</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goglcb5ptm7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1lea7s7</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzqjpizgsm7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1le9wc9</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Gold flake marble matcha nails</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le9wc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1le9r4v</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Japanese nail salon</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46qwubu2nm7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1le9e66</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Best OTC press ons?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1le9e66/best_otc_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1le9cuj</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Pink fun! 🩷</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uck7yxjim7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1le8fud</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Is this contract dermatitis or something else?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le8fud</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1le8iv1</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le8iv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1le8ppa</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Two as one?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dblav62hbm7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1le8z6d</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Nail fungus?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le8z6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1le8tlm</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>grad nails! 👩🏻‍🎓🎓</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yx2jqbncm7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1le8qdu</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Birthday nails 💛✨</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl21ff3obm7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1le8omn</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Big love for Mr. Bug on my new set!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le8omn</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1le8boo</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>One of my favorite sets</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vfhn0ge7m7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1le4lzy</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Nail’s in need of care</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91iuibhd8l7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1le89c8</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Makes me think of lucite purses, love!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le89c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1le86f1</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>For my trip to Colorado</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le86f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1le81sg</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>I think they’re cute!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9b2f18li4m7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1le7vf2</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Shorter nail bed girlies 🫶🏻 - @NailzByPriya</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le7vf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1le7d0a</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>I did freehand enameling with daisies</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fol4l52lxl7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1le75fz</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Pride nails (but also summer) 🧡🤍🩷🐬</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le75fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1le6rv5</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>My fav set</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fb22712sl7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1le6nbd</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>The most PERFECT tiny frenchies I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6g2olrvql7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1le6hy0</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Might be THE cutest press ons I’ve ever found</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw29o9dipl7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1le6e7h</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Decided to try my hand at press-ons today after seeing these as acrylics online :) new hobby 🔓</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9pn38viol7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1le6bq4</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Progressss</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le6bq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1le4flv</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Inspired by the girl on here who had the textured rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le4flv</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1le5bwg</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Gel mani post-acrylics removal 💖</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le5bwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1le5rgl</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Shellac Manicure - @NailzByPriya 💜</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le5rgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1le5e6i</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>My new nail tech!!!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv6a5c4ffl7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1le58ym</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>birthday nails 😊</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0r2xthl4el7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1le52dq</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Summer Fun!!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3m94hogcl7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1le51v5</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Gel X chrome french fresh set with a cute little flower 🌸</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xffzt40ccl7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1le4xvv</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Gel X to Regular Gel?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1le4xvv/gel_x_to_regular_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1le4jo6</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>what’s this style of nail color/polish called?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le4jo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1le4hhl</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>first set thats actually being sold. What do we think?? Honestly is always welcome ❤️ She was going for a Y2K look! 💓👌🏻</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7z9f85677l7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1le4bbo</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>thought you guys might appreciate &lt;3</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le4bbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1le49km</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>I'm sad these had to go</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le49km</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1le3iwo</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Help me pick my nails for this week</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le3iwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1le464t</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Chrome pickle nails 🥒✨</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le464t</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1le3m6z</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>natural acrylic overlay!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zesi99yjzk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1le3h2z</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>What’s the difference between a gel extension set and a tip set with gel polish</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rix851rbyk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1le3bxv</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>New nails 😁</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epkjqca3xk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1le3bkt</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>I made the Butter Yellow work🌺</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5g35dn50xk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1le33vg</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Press-on Nails for Prom</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1le33vg/presson_nails_for_prom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1le38lt</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Best way to make press ons last longer?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1le38lt/best_way_to_make_press_ons_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1le36oe</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Assignment Understood 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le36oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1le30p0</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Fresh set, simple but fabulous 💅🏻✨️</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j45re6rduk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1le2top</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>longer nails than i’m used to but i love them!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmtnxrkssk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1le2qy8</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Love seeing everyone’s pride sets!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/megeqm95sk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1le120c</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Best at home nail options</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1le120c/best_at_home_nail_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1le1inh</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>How are people doing designs with gel nails, when the stuff is so THICK?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1le1inh/how_are_people_doing_designs_with_gel_nails_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1le1el2</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>My mani is magically delicious for pride!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le1el2</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1le1apz</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Rate my handmade press on nails  🫣</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le1apz</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1le1821</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>What nail shape would be most flattering for my hands? Please help!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ggpt2ptfk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1le10xm</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>I’ll just look at these and pretend I’m at the beach 🌊🐚</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le10xm</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1le103d</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Love this color for summer</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le103d</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1le004q</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Ring of Fire is...spicy.</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my6zzxvi6k7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ldzj1c</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>More Pride nails</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rwxc9pz2k7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ldzifn</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Tried my hand at the fruit/ceramic inspo nail art</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cna2h3v2k7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1le0sb6</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>red marble nails!</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le0sb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1le0m3m</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Question about UV</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1le0m3m/question_about_uv/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ldzwf5</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Need them off</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzy9xvmr5k7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ldzrgh</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Another cute summer slay</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldzrgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ldzmak</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Assignment Understood!(Pinterest inspo last photo)</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldzmak</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ldz9dc</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Matching my toes to my fingers, I love this color so much right now.</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8d2e4qz0k7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ldzcbv</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Still obsessed with this set 💅🏽</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldzcbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ldyxrt</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Picture drop! I only do manicures polish. I love nail art and have been successful with polish art.  Can you share your polish art nails?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ldyxrt/picture_drop_i_only_do_manicures_polish_i_love/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ldyiui</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Tried a new shape!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k178au7rvj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ldy8lj</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Hello summer! 🌸🌼</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldy8lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1ldxksa</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Can I use UV curing nail glue as a “top coat”?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f80g40i0pj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1ldxbug</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Got these for the Beyoncé concert 🌟</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/voatkgpanj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1ldx3hw</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>My first experiment in the style of Cyber Y2K</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldx3hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ldwz2v</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>HOW DO I TAKE THESE OFF??</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq5nfwqtkj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ldwxu7</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Hi! I would just like some feedback 🙃</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldwxu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1ldwzip</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Who says you can’t ride and still be a little girly?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zndvouwkj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1ldwouh</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Pokemon Nailart</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldwouh</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ldwnui</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>How do I stop this black gunk from appearing under my nails?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xufeqg3mij7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ldwipq</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Koi pond nails</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldwipq</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ldwl66</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Happy Pride! 🧡🤍🩷</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldwl66</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1ldw2lm</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>What’s the best way to fix this?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldw2lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1ldw307</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Gel X DIY Summer</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldw307</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1ldv7q3</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>First summer set trying to be creative 💜💕</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldv7q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1ldtx11</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>So disappointed</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldtx11</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1ldu2w8</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>TW. HEARTBREAK. My first time having long natural nails.  Tl;dr vent post</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k39gscg11j7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1lduqzl</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Blue Chrome  💙</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lduqzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ldufb1</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Are these bad as I think they are ? I'm unhappy with my middle finger feels its uneven or too thick..please Any opinions?!</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldufb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1lduato</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>First manicure by me in home</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsp13xjh2j7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ldtx4o</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>I'm obsessed with this shellac colour 😍💅</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pozdrkzwzi7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ldo5kw</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Biab nail chipped and its orange underneath? Is this normal?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0nos43ewh7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1ldscor</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Can I use rubber top coat to encapsulate glitters/stud?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ldscor/can_i_use_rubber_top_coat_to_encapsulate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ldt5c8</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Getting used to polygel</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldt5c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ldsyn5</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>I'm devastated</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60zrc1m9ti7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1ldsxi6</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>New nails match my mimosa!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5hcscq5ti7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1leafuu</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Bees Knees Question!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1leafuu/bees_knees_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1le8gmy</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Nude/Pink Recommendations for my nail beds</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/512r3fyt8m7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1le9bg4</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>I feel ethereal</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8bfnzmpthm7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1le80nw</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Color club question</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le80nw/color_club_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1le7k4f</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>First BKL and WHAT IS THIS SORCERY</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le7k4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1le6pnw</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>The little edge breaks are killing me</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqsxlfghrl7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1le6pkl</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>cirque colors quality?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le6pkl/cirque_colors_quality/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1le6l9j</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>$3 Nail Polish?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s2ck2tcql7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1le6k0o</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>BKL - Your Soul is my Soul</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/49cyvsx0ql7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1le6k1m</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Give me your honest reviews on the Holo Taco cuticle oil pen</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le6k1m/give_me_your_honest_reviews_on_the_holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1le6ake</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Is she orange? Is she pink? I think…coral!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le6ake</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1le692g</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>This jelly makes me think of lucite purses!</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le692g</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1le57t5</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>birthday nails 😊 (contains a pr item)</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oav60rgtdl7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1le4ybo</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>the purple of my dreams</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5bep9ppfbl7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1le4w9z</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Recently developing gel allergy - help needed</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le4w9z/recently_developing_gel_allergy_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1le4s8w</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>I cannot find a glass nail file that compares in quality to the one I have now</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le4s8w/i_cannot_find_a_glass_nail_file_that_compares_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1le4luf</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Struggling with GITD from Zombie Claw</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le4luf</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1le47yl</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>First foray into ombres and chrome powders</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le47yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1le3j4x</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>How to get velvet magnetized nails less patchy?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le3j4x/how_to_get_velvet_magnetized_nails_less_patchy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1le3gwm</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Accidental mermaid</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le3gwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1le2vbq</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>sunlit skittles! 🖤</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le2vbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1le2na8</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>I'm ready to give up on reg polish</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le2na8/im_ready_to_give_up_on_reg_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1le2a09</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Thicker polish brands</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7yjfhdn7ok7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1le1zt6</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>My first Polished for Days!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le1zt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1le1shd</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>(ISO ) shake your shamrock Dreamland laquer</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le1shd/iso_shake_your_shamrock_dreamland_laquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1lduuzz</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Dupes or Sisters?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lduuzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1lduo7m</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Ethereal lacquer moon water skittle!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lduo7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1le1fmj</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>💚🤍🩶🖤Agender and Pan Pride💗💛💙</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le1fmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1le1e8o</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Ethereal moon water collection</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le1e8o/ethereal_moon_water_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1le0vak</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Cracked  vs Mooncat</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mova8ba2dk7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1le0n6b</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>100% Acetone-free remover that works fast?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le0n6b/100_acetonefree_remover_that_works_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1le04mq</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>What things have you ruined with acetone or polish?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1le04mq/what_things_have_you_ruined_with_acetone_or_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ldzlyk</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Using cuticle nippers on dark cuticles</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldzlyk/using_cuticle_nippers_on_dark_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ldywto</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Lurid Barbed Beauty</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldywto</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ldyw4m</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Do I need the HT pastel linear rainbow collection?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldyw4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ldytqk</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Where to buy thermal nail varnish in the uk?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldytqk/where_to_buy_thermal_nail_varnish_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ldypvw</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Suggestions on Nail Shape?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldypvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1ldydzy</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>I would like reviews and suggestions for a white / milky polish with a very strong red or pink glowy shimmer please!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptriysbtuj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ldv77e</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Halo Taco Lite link vs Mooncat River Styx</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldv77e/halo_taco_lite_link_vs_mooncat_river_styx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ldxw49</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Mooncat “The Sea Between Us” looks like a blue opal! 🧜🏼‍♀️💎🦋</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bff3c2j9rj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ldxj4l</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Nail art as art/nail art is art</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n50fxx9noj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ldxce3</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Reorganized and swatched all my polishes 🫡</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldxce3</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ldx730</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>ManiMod discount code</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldx730/manimod_discount_code/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1ldx6hi</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>ILNP Nostalgia is the jewel beetle polish of my dreams🪲</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p145zzlamj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1ldx0x6</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Jellies really brighten up a dark manicure</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sbwxhb7lj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1ldwww3</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>They're sooooo beautiful 😍</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nff6c4ekj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1ldwwcd</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Have any brands released their PPU rewind picks?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldwwcd/have_any_brands_released_their_ppu_rewind_picks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1ldw015</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Swapping Barbie Heads &amp; Bodies🩷</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/30lexmrwdj7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1ldvyd8</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Cool Waters + bonus ster pic!</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldvyd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1ldv7nk</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Korean Polish brands?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldv7nk/korean_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1lduqtg</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>You Threw Off My Groove 💙</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lduqtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1ldup8a</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>This weeks haul 😭</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdxhm4i55j7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ldub5m</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>So so good!</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/svc8h1fi2j7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ldtsrb</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>I love when magnetics</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wg1vua43zi7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1ldtomy</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Removing water-based paint without ruining mani?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nspcvdpbxi7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ldtnc5</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Any other thermal polish lovers??</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldtnc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ldt083</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Broke a nail but not the polish lol</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjlkbi6pti7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1ldsuoz</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Happily influenced</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l2qru1wisi7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ldsuy4</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Can I use rubber top coat to encapsulate small glitters/studs?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldsuy4/can_i_use_rubber_top_coat_to_encapsulate_small/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ldsrl8</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>EdM Second Chance or DVN I'd Let Him Eat Crackers in My Bed vs HT Vitamin Glow</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldsrl8/edm_second_chance_or_dvn_id_let_him_eat_crackers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ldsefm</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Cracked- Pond Stew 🦆🩵🍲</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldsefm</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1lds5gy</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Flash vs sunlight</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a3ori6gzni7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ldrysc</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Rainbow nails 🌈</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldrysc</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ldrynp</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>i think i have a new favorite child</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldrynp</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ldrxhs</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Fancy Gloss thermals arrived!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldrxhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ldrtnz</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Shifty Goodness!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebwndidsli7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ldrag4</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Fancy Gloss ❤️</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b49ia305ii7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ldr4st</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>I could not decide, so I used both and attempted to connect them via ombré in the middle</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp6i6s22hi7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ldr4mm</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Gel polish on top of lacquer removal?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldr4mm/gel_polish_on_top_of_lacquer_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ldqwt3</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>eat glass</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7i39r12mfi7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ldqhyu</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Beaux Rêves - The Little Prince</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tacmbh1rci7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ldpn95</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Phoenix Indie - AKasha</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldpn95</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ldpitk</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>I finally finished my project!!</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldpitk</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ldpe0u</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>can’t believe this isn’t gel</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldpe0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ldpcov</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Just some advice please 🙏</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldpcov/just_some_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ldp08d</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Neons…</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t48aduag2i7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ldokgr</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>ILNP Magnetics Recommendations</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldokgr/ilnp_magnetics_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ldohlg</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>A classic red in the lab 💅</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gx4akrrpyh7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ldnu6q</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>How to achieve this S shape effect in the Psilocybin Swatches?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ldnu6q/how_to_achieve_this_s_shape_effect_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ldm2za</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Has this notice always been on the Mooncat website?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjoxkfj6gh7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1ldltj0</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈💙🩵AroAce Pride Flag💛🧡🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldltj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ldlkrw</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>My first Revlon… does NOT disappoint! 💅🏽💖🌸</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/daejvd4ubh7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1ldlct3</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Tips for Good Skittles?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldlct3</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1ldlaa0</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldlaa0</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ldkv3d</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Finally tried fairy dust 🧚‍♀️✨️</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldkv3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1ldjdos</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Looking for a modern version of this polish</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdy4k6yxpg7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1ldhp1x</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Trans Pride!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldhp1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1le9pfm</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Redesign of a set I did over 3 years ago</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le9pfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1le6g5w</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Help me w my nail design!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le6g5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1le6efb</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>may/june dump</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le6efb</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1le543p</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>It’s been a while since I last posted but I still think I’m starting to improve.</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le543p</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1le4wip</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Looking to get into nail art</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1le4wip/looking_to_get_into_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1le2e1y</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Halsey set!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le2e1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1le1d10</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Wore these to my first day of Paul Mitchell the Nail School 💅🏼</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1le1d10</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1ldyq5s</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Nail school is fun 🫠</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnnqyj87xj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1ldxbfm</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>As a beginner, I’m so happy with these!</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6g33am7nj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1ldvw36</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Gel X DIY Summer</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldvw36</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1ldvf6p</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>bi pride flag set🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlluzlb6aj7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1ldv5eg</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Progression</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lshsgia8j7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1ldqwzw</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>My cute summer cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7yx6p8nfi7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1ldqtqz</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>First time I have some nails like that and I loved them</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hovksqxhei7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1ldq78y</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Rainbow candy nails for pride</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ldq78y</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ld97ux</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>SpongeBobby 🧽</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yva8g481sd7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1lddjqo</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Should I do a bouquet of roses?🌹</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ucafq55uue7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1ldktlx</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evtm33bl4h7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1lcqi6z</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Temu nail products</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lcqi6z/temu_nail_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1lci2gr</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Clowning around with these nails 🎪💅</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m038wrnwd77f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1lbq6ir</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>A shot of tequila please!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxysey8za07f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1lbf5sq</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>New to nail art! Opinions/Advice?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lbf5sq</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1la92yj</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Fresh pride set!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch1yv5qa3n6f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1la5164</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Who would wear these claws? Took me all day since I had to build them from scratch 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1la5164</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun 19 08:13:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_22.xlsx
+++ b/data/collected_data/2025_06_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C714"/>
+  <dimension ref="A1:C901"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12571,6 +12571,3185 @@
         </is>
       </c>
     </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1lf4on9</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Thoughts on length and shape please</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf4on9</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1lf485n</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Got 3d press ons applied in store but most popped off in 24 hours, help please!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lf485n/got_3d_press_ons_applied_in_store_but_most_popped/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1lf426k</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>My new favorite</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xi75r4wyt7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1lf3s9n</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>what do you think of my vacation nails!!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8cap9fqvt7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1lf3ij2</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Gel or acrylic for vacation?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lf3ij2/gel_or_acrylic_for_vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1lf2nu1</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>how do i get better at using my left hand for doing my own nails?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lf2nu1/how_do_i_get_better_at_using_my_left_hand_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1lf32r8</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>You all will understand what upsets me most about this</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rhgc80pnt7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1lf2p2x</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Why do hard gel or polygel nails always break in the same place?!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2x1fh9ijt7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1lf2hat</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>French + glitter</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf2hat</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1lf29z7</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Critique please</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf29z7</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1lf1zi2</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Green franch nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf1zi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1lf1nry</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Guy getting his first mani/pedi</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lf1nry/guy_getting_his_first_manipedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1lf1ms1</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Sharpicure</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7otverc8t7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1lf1fvc</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>happy pride! just got my first gel kit!</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf1fvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1lf1ikg</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>why is there such a big dip right here</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf1ikg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1lf1fal</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>2 week old gel manicure</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aj2pzco76t7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1lf15rr</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>nail day!!!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxef8jmn3t7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1lf12l0</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Cateye!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf12l0</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1lf0net</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Random designs but I like them</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf0net</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1lf0a9q</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Dream Within A Dream</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ke4nzk6avs7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1lf03x3</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Ocean blue cat eye and gold chrome.</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r21znuhnts7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1lezq2p</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>This isn’t polish, it’s black glitter acrylic 😩 My fave nails I’ve had in ages!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bvso56g3qs7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1lexn3b</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Teenage me is happy, adult me is also happy</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6r7fc4dl7s7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1lez9dn</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Love it！</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6f8o6evxls7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1lez0gm</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Short colorful gel overlay set</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lez0gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1leymte</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Can I still get my toes done with a blue nail</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1leymte/can_i_still_get_my_toes_done_with_a_blue_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1leyivu</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Cherries 🍒🥲</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42q8v9ygfs7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1leyd6a</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Self-made nude nails, I love it！</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t87943s1es7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1ley8ih</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Gel nails for those who bite their nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ley8ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1ley55p</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>I made these leaves by hand and I hope you like them</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsqyz5t1cs7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1ley4td</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>First time doing my own dip nails</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6z7yro7zbs7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1lexyzt</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>aura nails with some charms!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntqf9tcjas7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1lexm2g</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6cr5ucb7s7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1lexebv</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Need advice on how to keep my nails on.</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lexebv</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1lex1ob</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Me: “Can you do *insert insane idea here*” My Nail Tech: “Bet.”</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lex1ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1levze3</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>How do we feel about the shape?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlut0svctr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1lew8vl</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>$7 press ons????</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kthksarkvr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1levu6f</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Watercolor, freehand🩶</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94ogisv3sr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1levrzs</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>First time doing Gel X/nail art!</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1levrzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1levhhs</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>In love with my new set 🥹</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1levhhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1lev9ub</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>green chrome nails so shiny i caught myself staring like twice</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3iwvm2lnr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1lev5xz</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Cluthching my pearl nails</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lev5xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1letlcp</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Show me your Pride nails! 🌈</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1letlcp/show_me_your_pride_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1leu16m</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>DabiHawks Nail Set</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5284mctdr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1leu0dh</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Classic red!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ix0k84ndr7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1letzzu</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Justifiable reason to ghost a nail artist?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1letzzu/justifiable_reason_to_ghost_a_nail_artist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1letddx</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>I am obsessed</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uxpz83qu8r7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1let4ot</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Help me fix my nails</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fsgn2f217r7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1let06b</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My nail tech’s take on the butter yellow trend 🧈</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pd08hb06r7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1lesr0q</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>First Attempt at Cat Eye Nails by Me!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/suixbgd94r7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1lesm2n</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Peeling fingers, help!</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lesm2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1lesehu</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Your go-to magnetic gel polish brand (and a question about magnet strength)</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lesehu/your_goto_magnetic_gel_polish_brand_and_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1les7y5</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Yellow French Chrome</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okynw18h0r7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1les3q5</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>My New Set!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1les3q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1ler50n</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I love doing my nails 💓</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ler50n</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1leqy4b</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>I need alternatives to salon nails to save money</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1leqy4b/i_need_alternatives_to_salon_nails_to_save_money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1leqsy7</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Shrimp cocktail nail set 🦐🍋</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63i7pjy8qq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1leqrhx</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My New manicure</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnln9dlxpq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1leqlw7</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>A little late</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leqlw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1leqgwl</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Western vibes for a local drag queen🩵🐮✨</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aw0fas6unq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1leq8hr</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>What do u think?? I like them but i feel like it’s too long, I am not used to this length 🫣</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmim06c6mq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1lepw9e</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>How much would you charge?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aelrzfcsjq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1lepr41</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Beach towel vibes 🌊</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc1pw98siq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1lepdlo</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>When you don’t have access to detailing brushes…</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbisaw18gq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1lepcji</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Must dos at home for pre-engagement nails?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lepcji/must_dos_at_home_for_preengagement_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1lep6mc</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>My non-gel purple/magenta glass nails!  Getting the hang of light chasing technique</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yccuqtlueq7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1leoxhl</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Cuticles cut badly after nail appointment</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mi325f1dq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1lep0oz</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Wondering what to do next...</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lep0oz/wondering_what_to_do_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1leozdw</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Blue chrome 🩵</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leozdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1leow0h</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Russian Manicure + Gel</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leow0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1leoofc</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>How bad did this come out?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z7hwababq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1leoms2</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Bio gel nails</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leoms2</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1leomji</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>🩵</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/573vr2wxaq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1leobdi</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Help with Nail Shape/Length</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10vgo35o8q7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1lenwpk</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Which nail shape/length would best suit my hands?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1s9vus8y5q7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1leni1h</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>watermelon nails for summer :)</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8iri3q03q7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1lengw8</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>HELP! engagement nails!!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lengw8/help_engagement_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1len43l</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Keep my nails healthy with glue</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1len43l/keep_my_nails_healthy_with_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1len8dc</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>pink marble set 💖</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpc2ohx81q7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1lemmmu</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Are these rings of fire?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/516kfns3xp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1lemag5</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Had a bad day and got my dream nails done</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lemag5</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1lem0t4</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Improve natural nails, especially the tips</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lem0t4</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1lejsgv</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>First time getting nails done in years, I have questions</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lejsgv/first_time_getting_nails_done_in_years_i_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1lekgpl</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>I need help</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mci8hn2ip7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1leeobx</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>How do I stop biting my nails?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leeobx</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1lel9eg</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>What Is This Called? Inspo pics from @o.round1128 and @m.petitnail on Instagram and An Cherir Nail Salon</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lel9eg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1lell94</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Boat trip</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gusbpqypp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1lekvdz</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Learning how to do my own gel nails to kick a nail biting habit!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erx051txkp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1lektc7</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Lecenté fusion builder gel</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lektc7/lecenté_fusion_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1leksyx</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Funny Bunny will never let me down</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncq86johkp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1leksgs</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>My first blue manicure!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leksgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1lekm8f</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>The details is on fireee</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0js15aa3jp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1lekhup</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obnnpaiaip7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1lejmu7</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>New nails, is the price reasonable?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b29kzxo7cp7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1lejivc</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Have you ever had such a horrible experience at a salon that you said, Fine. I will just do this myself.</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xyzyv5abp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1lece83</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Been doing my own nails trying to get better at it. How do you think I'm doing &amp; feel free to give advice. Thanks:)</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lece83</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1lecryk</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Is it normal for bio gel to lift like this after 2-3 weeks?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lecryk</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1leg2bf</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Need advice, please — wrecked cuticles?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leg2bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1leel2e</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Patriotic nails</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbiq0wyh7o7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1leddo4</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>would these be cute? any critiques?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwm8pmnlun7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1lf2t85</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Mooncat A Midsummer's Dream OPI dupe name????</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lf2t85/mooncat_a_midsummers_dream_opi_dupe_name/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1lf30jn</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>LynBdesigns first order!</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lf30jn/lynbdesigns_first_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1lf2lbe</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Chrome powder over regular polish</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n3xbapfdit7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1lf285p</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>🌳No Shrubs🌳</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf285p</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1lf26if</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Dupe Recs PLEASE!!!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2o9sbk0et7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1lf1trf</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>This magnetic only looks good before top coat?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bnjhbi8dat7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1lf0ha5</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Cosmic Polish is shipping to a bunch of countries!</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0xf11f3xs7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1leze70</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Looking for nail color</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1leze70/looking_for_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1lez3yt</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Magnetic Toppers are a Godsend</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lez3yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1leyu9j</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Essie bermuda shorts dupe</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2hwx6h9is7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1leygdl</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Sparkles</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tr93y49ues7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1ley09q</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Nonbinary stripes and rainow skittle</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ley09q</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1lexxb2</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Rainbow and nail stickers on glitter</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lexxb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1lexr9f</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>My gym has the BEST lighting for sparkles!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0611y98n8s7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1lexh66</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>My bathroom/shower is becoming my favorite space to enjoy my nails</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lexh66</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1lexg3x</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Help Me Find My Old Polish!!!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lexg3x/help_me_find_my_old_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1lewqr1</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Pan🩷💛🩵 and Bi🩷💜💙 nails in honor of my friends!!</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lewqr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1lewiru</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Crack - How would I repair?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lewiru</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1lewik5</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Back to basics</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lewik5</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1lew8if</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>ILNP Shimmer Skittle!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lew8if</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1lew0r1</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Just getting into nail stickers gonna have to buy more</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9otxw6wntr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1levzrq</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>LBOH confusion...</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1levzrq/lboh_confusion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1leupal</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Fancy Gloss 'Drift Dream' as a Ribbit Ribbit Dupe. Not quite, but close enough for me.</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcami3iehr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1leungq</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>What are your favourites from Lurid?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1leungq/what_are_your_favourites_from_lurid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1leulbq</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Alice appreciation post 🌥️🏙️🩵</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leulbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1leu59e</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>My pride heart mani</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv5wmh9ydr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1letw9s</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>New Lurid x Cracked collab a possible dupe for Mooncat Plankton? What do you think?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1letw9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1letu79</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>"Blood on the Ground!"</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1letu79</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1letqjn</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Glow-In-The-Dark Polish is NOT forgiving</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1letqjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1letkv1</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Fun Lacquer - Comfort Zone</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1letkv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1letjmq</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Tranquil Tide</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1letjmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1let8rd</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>🐍 slithery little snake 🐍</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1let8rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1lesvk1</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>For pride, I went with 🎶 hearts, stars, horseshoes, clovers, and blue moons, pots of gold and rainbows, and tasty red balloons 🎵</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lesvk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1lesgyx</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I struggle with the magnetic polishes but this is the best I've gotten em to look so far</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lesgyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1lesejo</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Using cuticle oil for the first time</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lesejo</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1les3lh</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Is this due to top coat drying out?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0uhl1rlzq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1les0az</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>OPI Lacquer/Laquer Do You Sea What I Sea? (OP)</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2ozltuyyq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1leryx0</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>BKL question</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1leryx0/bkl_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1ler77d</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Dupe for Ethereal’s ACOTAR mystery?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ler77d</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1ler3mn</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Summer Jinx</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ler3mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1ler2o9</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Shimmery rainbow gradient for Pride Month 🌈✨️</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ler2o9</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1ler2nk</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Most long-lasting polish brand?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ler2nk/most_longlasting_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1lepvzk</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Pinterest is the easy cataloguing solution I was looking for this whole time</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lepvzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1lepu51</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>losing you yellow</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/715i71hdjq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1leov51</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Fancy Gloss order has arrived!</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leov51</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1leotwa</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Shimmer on Shimmer</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awxfg99vaq7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1leokjs</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>I was feeling sad so I painted a lil friend</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leokjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1leoj2d</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>My non-gel purple/magenta glass nails!  Getting the hang of light chasing technique</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wx170y58aq7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1leo4f6</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Dinaco Blue Nails</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leo4f6</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1leny55</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Blue Ombre Skittles Mani</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9af8rkk76q7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1lenxrt</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Show me your manicure space/setup!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lenxrt/show_me_your_manicure_spacesetup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1lenaf6</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>My absolute favorite glowy polish!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lenaf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1lemnkk</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Did my mom’s nails</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8y9zsk9xp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1lemkm6</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>The dry brushing continues</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/LPIaSM5.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1lem8vj</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>recommend me a polish like this please?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lem8vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1lem8p8</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Does a peely base help with removing polishes with large flakies and glitters?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lem8p8/does_a_peely_base_help_with_removing_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1lem4h0</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Bewitched by Coven Spell</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lem4h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1lek1xc</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Hypnosis is hypnotic</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n50m2jg2fp7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1lejz70</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>BACK TO BACK!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lejz70</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1lejqgv</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Plant Aunt💚</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lejqgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1lejkfd</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>What do you do with product you know you won't use?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lejkfd/what_do_you_do_with_product_you_know_you_wont_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1lej77t</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I Love this Subreddit ft. Deep Space</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/viyfh6fa5p7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1leidp5</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Using Lacquer for press on nail art?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6innofz63p7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1leiba2</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Drugstore Base coat that won't make Nails Peel?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1leiba2/drugstore_base_coat_that_wont_make_nails_peel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1lehdpn</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>🏳️‍⚧️🩵🤍Transgender Pride Flag🤍🩷🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lehdpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1leh9fg</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Magnetic forays 🧲</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leh9fg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1leh1f8</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>We gather here today to mourn our Dearly Departed ⚰️🪦🥀</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvt70962so7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1legnp9</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Brightening up the workplace</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz66vkm2qo7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1leg06h</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>I started doing my own nails and wanted to share my progress :)</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leg06h</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1leg05b</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Not sure if this suits me but pretty on its own</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leg05b</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1lef7dk</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Tips on swatching magnetic polishes more efficiently?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lef7dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1lebrj2</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Palette London? I'd love to see what they look like on</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lebrj2/palette_london_id_love_to_see_what_they_look_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1lf472k</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>My third DIY nails at home attempt</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf472k</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1lf3tcn</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>First time using 3D gel for the flower 🙈</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kbpail2wt7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1lf17wr</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>4th of july press on</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8q7k1ge84t7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1lexjkl</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Still not over this set I did</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lexjkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1lexidl</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Nails I do on myself as a nail tech</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lexidl</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1lev7ex</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Help!! My 3d sculpting gel is too sticky!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lev7ex/help_my_3d_sculpting_gel_is_too_sticky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1leu4nu</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Made a timelapse video</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4w4wjmkger7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1letzii</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>DabiHawks Set</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqoae2igdr7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1lemtes</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Vacation nails!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lemtes</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1lemrfw</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Take me to your leader 👽</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lemrfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1leknto</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>🎶 Be Who You Are For Your Priiiiideeee 🎶</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1leknto</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1lejsji</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Anyone help with how to hand draw cherries a little better? I always struggle</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bv1s81cdp7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1legaql</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>This group taught me how to stamp nails, so I thought I'd return the favor with a tutorial and swatches</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvyaqmb5no7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1leftn3</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Started doing my own nails 3 months ago and i wanted to share my progress :)</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1leftn3/started_doing_my_own_nails_3_months_ago_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1led77l</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>My first set of holiday nails ☀️</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ras8xgelsn7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun 20 08:12:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_22.xlsx
+++ b/data/collected_data/2025_06_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C901"/>
+  <dimension ref="A1:C1083"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15750,6 +15750,3100 @@
         </is>
       </c>
     </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1lfx86g</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Hey girlies!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cj5ve8rd318f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1lfwuh0</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>What nail shape and colors/style would suit my skin tone? (also sorry my nails are hideous rn i just showered 😬)</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox7lqgzny08f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1lfw69n</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Need advice on my new acrylic set, please!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jtba3ba6r08f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1lfvv2s</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Fruit punch 🩶</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agw9w0lsn08f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1lfvui3</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>I don’t think it’s supposed to happen</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jy6v6x8mn08f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1lfvgl0</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Navy 💙</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oui2kvbgj08f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1lfva70</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>accidentally built a couple of my fingers with base gel instead of builder gel 🥲</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn4lf3tkh08f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1lfmagi</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>4th time ever doing dip</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0w0gppx9y7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1lfq2pq</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Is it too much to expect my nail tech to make my nails generally the same length and shape?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfq2pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1lfv0cw</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>polish recs for at home pedicure?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfv0cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1lfuzhn</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfuzhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1lfustb</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Fruit basket nails anyone?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfustb</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1lfno5v</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>I'm a climber, and I want a manicure for a wedding. What do I need to do to prepare?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfno5v/im_a_climber_and_i_want_a_manicure_for_a_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1lfqx37</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Helppppp! Ewww.</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfqx37</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1lfr1bc</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>How do I heal my cuticles/the skin around my nails?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfr1bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1lfroz6</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Best nail shape for me?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfroz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1lft1ua</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lft1ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1lfto1t</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Orange inspired nails today.</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im74fgze108f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1lfuhk6</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>happy pride 🌈</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfuhk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1lfu7ku</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>DIY press ons for concert</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfu7ku</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1lftkhl</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Frenchies✨</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lftkhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1lftimt</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>🐠🪼🐚🪸</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lftimt</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1lft3to</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Thoughts on this shape? Never did oval</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eaio094wz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1lfszy7</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Opinions?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uwzjqs2vz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1lfsybl</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Dip nails with tips</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfsybl/dip_nails_with_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1lfsrnb</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Happy Pride set 💜🩵🩷💛💚</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghscd5nvsz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1lfslou</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Summer nails for my trip to Italy</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1ignl5crz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1lfsi07</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Pride nails (I know I’m late lol)</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhf3f4teqz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1lfsfxf</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Press on's french tips🤍</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfsfxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1lfs91e</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Strawberries and cream</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbxlcv55oz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1lfs780</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Fired A Client</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vndi79bonz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1lfs65f</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>🌸🤍 cat tail included in 2nd pic 🐈</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfs65f</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1lfrxtt</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>cutesy nails</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo7w1yv6lz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1lfrt8a</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Love the subtle ombre</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4deles6zjz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1lfrdvr</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Favorite sets</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfrdvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1lfrd4b</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Beneficial nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfrd4b/beneficial_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1lfr4q8</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>I ran out of plastic nails and decided to print this on cardstock. It works! All my chrome powders swatched over black gel polish</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfr4q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1lfr1bw</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>It was our first times doing at home GelX!!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3qqewgzcz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1lfqyek</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfqyek/how_did_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1lfquoq</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Something Cute</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfquoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1lfqtgq</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Love this new press on set from Mom!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n82itvj1bz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1lfqhn4</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Recent biab set 💛- @NailzByPriya</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpsi4aw48z7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1lfq9id</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Freehand tribal for my client!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qua2e856z7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1lfq9dx</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Press ons for under $5!! And anything else you can want for cheap!!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfq9dx/press_ons_for_under_5_and_anything_else_you_can/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1lfq4af</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Still loving the Russian manicures ✨</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dev7h3x4z7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1lfpopq</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Milky white nails + white chrome = ☺️</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1n7csru71z7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1lfpm2x</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>First time doing hard gel!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aij5d4dl0z7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1lfp58k</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Just made this set for my friend who is going to be a bridesmaid at a wedding 💙💙  Pastel Teal is the dress code:3</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab2let7hwy7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1lfp4sv</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Ocean Vibes🩵🧜🏾‍♀️</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rnqyihgwy7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1lfp1jv</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Uv gel for press ons - how to get them off?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfp1jv/uv_gel_for_press_ons_how_to_get_them_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1lfooz8</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Nail glue</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfooz8/nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1lfo5mv</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Birthday Set</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfo5mv</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1lfnw23</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Frosty Pink gel polish 💗💓🎀🩷🩰</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfnw23</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1lfn0vm</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Just Got New Nails Done 💅🏻</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1oea2tify7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1lfn0jf</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Vampy nails</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfn0jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1lflwda</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>My nails for pride month :D</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lflwda</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1lflux6</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Glazed 🍩</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biru5daq6y7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1lflszm</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Little fishies!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lflszm</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1lflsvz</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>New Manicure Feeling 🔥🕺🔥</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk3b7gza6y7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1lflonx</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Missing the daisies</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lflonx</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1lfl5o0</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfl5o0</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1lfkjx3</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Hello r/Nails😻I have 2 brand new still sealed bottles of OPI Affair in Red Square available for sale😽</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfkjx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1lfk54l</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>What nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfk54l</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1lfk3z1</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Cat eye 🪐</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6h19ilkrtx7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1lfk3od</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Tried coffin for the first time on my natural nails and I am a changed woman !!!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ffsbidptx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1lfjzan</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Sanitizer + Acrylic ?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfjzan/sanitizer_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1lfjw87</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>cat eye</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxjvgr35sx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1lfjvpd</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Neon summer set!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4p59gk1sx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1lfju9g</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Red tips over a glitter base, what do you think of this combo?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ziilzaqqrx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1lfjkze</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>My best press ons yet!</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xc4vllupx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1lfic5f</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Advice Needed</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfic5f/advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1lfhymf</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Onycholysis after using?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gw7mfigbex7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1lfj0wi</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Not sure what nails are best for me</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfj0wi</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1lfj7wv</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>what nail hardener actually works</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfj7wv/what_nail_hardener_actually_works/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1lfiyhm</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Are breaks necessary?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfiyhm/are_breaks_necessary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1lfix5s</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Can I fix my upturned nails?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfix5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1lfit5u</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Just spent four hours on my nails. Worth it!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfit5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1lfinug</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Todays client wanted 'små grodorna'. Midsummer tomorrow in sweden!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cck7d8rajx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1lfilnd</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Needed a palate cleanser from my usually detailed sets.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a0vbjcvix7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1lfi1g9</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>I did my nails. Do you like the cat eye effect?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/69ct36qmex7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1lfi0jf</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Tips for care and preparation for a manicure?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfi0jf/tips_for_care_and_preparation_for_a_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1lfhzgo</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Summer vacation means long nails💅🏻</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfhzgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1lfhq60</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>First time doing detailed nails and I’m in love!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfhq60</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1lfh9fy</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Are my nails supposed to be this straight?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfh9fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1lffeev</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Builder Gel Journey from a Nail Picker</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9dmfechww7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1lfgjzs</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Why did my top coat bubble?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfgjzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1lfgiwk</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Not too bad for a battery tech who does their own dip powder!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfgiwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1lfgcjk</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Found a rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p365ww033x7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1lfftjw</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>When not knowing which color to choose, cat eyes are always the best choice. How about you?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfftjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1lffmrv</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Bitchen baby.</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lffmrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1lffgr2</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>matched my graduation nails to my dress, what do you think?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c2h44lxww7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1lfelsq</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Obsessed with my polka dot nails 😍 Please ignore my broken camera lmao</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl897ttpqw7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1lfe7dz</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Complete amateur nails</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2csw0mfunw7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1lfa18r</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Nail shape</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfa18r</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1lfe5g5</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Birthday nails! (May 30th) ✨</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfe5g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1lf5aas</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Not my beat. But I was experimenting with chunky glitter for the first time. Lol</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lm06w56du7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1lfdvih</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Review for Chillhouse press-on nails</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfdvih</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1lfe487</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Soooo clean</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfe487</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1lf3oxo</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Nail extensions at home</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lf3oxo/nail_extensions_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1lfdq9b</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Gel reaction</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lfdq9b/gel_reaction/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1lfxvk8</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Summer Greens are out!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/im5il8msa18f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1lfwyns</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Another pride skittle</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfwyns</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1lfwpeb</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Asking for comparisons</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfwpeb/asking_for_comparisons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1lfwgki</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Press-On Troubleshooting</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfwgki/presson_troubleshooting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1lfwe6r</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Ocean Vibes</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/efdraubrt08f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1lfw9bn</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Pipe dreaming</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x0oavc1sq08f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1lfvgw2</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>ILNP Rock Candy🍭 + thank you my feral queen</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfvgw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1lfuya5</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>How do you pain your nails? One hand at a time? Both at once?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfuya5/how_do_you_pain_your_nails_one_hand_at_a_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1lftvcv</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Anyone order from KB shimmers/MoonCat or maniology to Canada lately?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lftvcv/anyone_order_from_kb_shimmersmooncat_or_maniology/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1lfu6cu</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Resin art or nail polish? 🤯😍</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mxk5kjap508f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1lfts6l</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Late to the party Pride chrome skittle 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp2aiqkj208f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1lfteim</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Post your swatches!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfteim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1lfsxpy</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>LaColors - soo many compliments from men women and children.</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfsxpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1lfspk8</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>My Advil Liquid Gel nails :D</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atewzc9csz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1lfsl20</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>A moment of silence for our fallen sister….</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o25rcd06rz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1lfsesy</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Splits/cracks in the sides of nails?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfsesy/splitscracks_in_the_sides_of_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1lfs1t9</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Can anyone recommend me a good white liner gel polish? Turns out normal white gel isn’t very pigmented lol</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad2m4z09mz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1lfrw7b</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Best polish brands for water marbling?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfrw7b/best_polish_brands_for_water_marbling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1lfrve7</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Question about Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfrve7/question_about_death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1lfrim4</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>sparkly pride nails</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfrgln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1lfrhqh</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>What was your game changer?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfrhqh/what_was_your_game_changer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1lfredw</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Sassy Sauce order</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfredw/sassy_sauce_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1lfqv45</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Where are my water babies at?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfqv45/where_are_my_water_babies_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1lfqv2d</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Reusing Press ons made of lacquer?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfqv2d/reusing_press_ons_made_of_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1lfpzrb</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Loving on Indomitable (Cursed pose in last pic)</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfpzrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1lfoubx</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Peel off base coats for those with peely nails</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfoubx/peel_off_base_coats_for_those_with_peely_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1lfobg9</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Balatron love</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5h4kzbcspy7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1lfoazb</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Can someone with a neon orange polish throw a blue shimmer topper over it?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfoazb/can_someone_with_a_neon_orange_polish_throw_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1lfn9td</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>ILNP - Pool Party and Fairy Dust!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e46h70khhy7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1lfmit3</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>🌈 spectra pride 🌈</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c79nfm9pby7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1lfm2u0</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>dupe for this phase of DVN blushin</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79kv7llc8y7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1lflu1y</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Help w ILNP Dollhouse + others</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lflu1y/help_w_ilnp_dollhouse_others/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1lfloo3</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>The difference between sun and shade for a linear holo</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfaji34g5y7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1lfli7k</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Is there a comprehensive list out there of Nail Savvy polish colors?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfli7k/is_there_a_comprehensive_list_out_there_of_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1lfjt5z</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Another Swatch Book 📖</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfjt5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1lfjquk</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Best indie brand for your fav purples, blues, and teals??</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfjquk/best_indie_brand_for_your_fav_purples_blues_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1lfji3x</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Happy Pride Y’All</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hic8g38apx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1lfjgky</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Little late, little gay, little halo</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n9ke7j6zox7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1lfj35v</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Cracked 🤫💜</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfj35v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1lfissg</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>I'm a shimmer convert</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uihhzfakx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1lfi732</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Tropical gradient</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0tmskczfx7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1lfhy97</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>This project is overwhelming!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0pr2nj8ex7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1lfhno5</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Day 8 of a Psilocybin mani 🤯🍄✨</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6yxd4nx5cx7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1lfh91u</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>🍉💅</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfh91u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1lffxmw</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Shroomdom 🍄</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03tbc8380x7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1lfh2e7</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>My "summer's almost started even though it's chilly enough to wear a sweater" nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfh2e7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1lfgulr</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Another blue I scored recently</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fy8yolag6x7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1lfgpub</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Topping a velvet mani with black flakes is my new fave thing to do</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rm20json5x7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1lfgcue</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Mint Green Calla Lily</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfgcue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1lfg750</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Most recent layering experiment</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfg750</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1lffntk</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Essie Mrs always right, I've found my red</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lffntk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1lfezyz</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Cat eye for beginners</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfezyz/cat_eye_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1lfdu8t</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Not sure if I like this colour on me, but I’m still proud of my first ombré nails</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfdu8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1lfdlt4</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Holo Taco Sparkling Spurs</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9tg0a9ijw7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1lfd1jf</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>First time posting nude without any colour</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuce8ztefw7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1lfd0wf</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Never knew drawing fish would would go so wrong…</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23c1cy2afw7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1lfck79</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>What brand should I try next?!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfck79/what_brand_should_i_try_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1lfc8mk</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Am I doing peely base coat wrong?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ychbidm9w7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1lfbf59</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>A smidge of spring spookiness!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfbf59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1lfbb9h</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>How similar is this to ILNP Vaporwave?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfbb9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1lfb04k</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>MC Sagebrush saved by FancyGloss</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfb04k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1lfaz2v</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>My Storage Box Color Is a Vibe - Looking for a Matching Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfaz2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1lfas3g</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Artemis death kiss 🤭</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfas3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1lfaqxz</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Maybe I should swatch all my magnetics like this from now on 🤔</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ju3n3r05uv7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1lfakxy</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>📋 Essie *Expressie* Shade List?</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lfakxy/essie_expressie_shade_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1lfajxd</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈🖤🩶Aromantic Pride Flag🤍💚🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfajxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1lf73bj</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Ideas for nail art?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lf73bj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1lf675s</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Can I mix these two together?</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn2yj774ou7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1lfvxfb</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>A little more of my beginning...</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ih8wh1wfo08f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1lfvc9o</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Obsessed with these holographic stiletto nails! Perfect summer vibes!</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ua24of16i08f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1lfv1og</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>French with cat's eye effect</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dj0dzhlsd08f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1lfv15h</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>New press on nail set!</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbnl6gqze08f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1lfse8s</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Did a holographic gel set with cat eye french tips for a friend - very much a newbie to nails</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om2c08mfpz7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1lfqhue</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Red and Gold Rosary📿💛</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfqhue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1lfq6i8</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Start doing them myself in January to save money. No regrets. #polygel</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfq6i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1lfpa48</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>New style</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjvkjoiewy7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1lfolqn</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Painting a Hercules set! Here is Meg and her hero 🥰</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1jk0m105sy7f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1lfo18q</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Checkers and flame nails</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikawysghny7f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1lflz55</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>My pride month nails!!</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lflz55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1lfjkhv</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>IT'S NOT EVEN MY FINAL FORM</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfjkhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1lfg432</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Starting in this world 💅</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjlb9qgf1x7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1lfcij9</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Based on Mabel's Sweaters</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfcij9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun 21 08:11:13 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_22.xlsx
+++ b/data/collected_data/2025_06_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1083"/>
+  <dimension ref="A1:C1287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18844,6 +18844,3474 @@
         </is>
       </c>
     </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1lgqqor</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Are these too long?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgqqor</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1lgq831</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Lisa Frank nails for summer</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgq831</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1lgpwr6</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Becoming a nail tech</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgpwr6/becoming_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1lgpmu0</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>What color is Iris from Love Islands French nail base?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgpmu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1lgnru1</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Are half moon nails a problem?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgnru1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1lgmopa</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>How do I stop chipping?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgmopa/how_do_i_stop_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1lgivma</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>I don’t know what I am doing</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sraoakp768f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1lggxh1</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Nail/finger suddenly feeling sensitive after 2 weeks of nail extensions</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lggxh1/nailfinger_suddenly_feeling_sensitive_after_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1lgpd1m</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>My first attempt at polygel</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgpd1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1lgoy6b</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>How to deal with hard cuticles?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bht3x2vpu78f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1lgohmm</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>A new set I did on myself!!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgohmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1lgobnu</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Biab in the sunlight ✨</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6mdzhkwn78f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1lgobiy</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>I had to do fruit &amp; am obsessed</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgobiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1lgo1qb</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>🌵</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsevmvm2l78f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1lgnsrn</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Disco nails</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgnsrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1lgn6kg</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Oranges! Gel x set</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wjzvno5c78f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1lgmu2n</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>i got this set today, and i think it’s my favorite of all time</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouahdmbn878f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1lgmn0p</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Birthday set done by me 🥰♊️</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhixo77r678f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1lgml9k</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Do men’s press-on nails exist? If so, are there any that actually fit wider nails and are easy to remove?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgml9k/do_mens_presson_nails_exist_if_so_are_there_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1lgm1t8</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>First time getting my nails done</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgm1t8/first_time_getting_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1lglc8f</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Alien candy nails 👽🍭✨</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lglc8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1lgl3gp</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Just got these done 4 hours ago</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0prscl1s68f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1lgl0fy</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Manicure advice for wedding</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgl0fy/manicure_advice_for_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1lgkyva</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Some press ons I’ve made so far this year</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgkyva</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1lgktcl</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>pride nails!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgktcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1lgkt7a</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Short nail girlie with longer french tips and i cant type anymore😝😝</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sm4da8ap68f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1lgkf79</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>First time acrylics on weak nails. Good/bad idea?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgkf79/first_time_acrylics_on_weak_nails_goodbad_idea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1lgkc3b</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>First time doing my own hard gel nails - tips welcome!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrvg7yrvk68f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1lgkay0</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Koi pond</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgkay0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1lgfoac</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>How can I avoid this bad lines on the edges when it grows</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgfoac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1lgirhx</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>first time posting 💖</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pty592q668f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1lgists</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Gel nails at home</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgists/gel_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1lgi8g9</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Just got my order from Emily de Molly and it's so good. 💜 I love her polishes! 😍</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbry6ova268f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1lgjgm2</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Oddity nails</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f730ppxsc68f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1lgizpm</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Armor nails</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ce4twjvm868f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1lgix6e</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Strawberries 🍓</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu18ffn2868f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1lgiw02</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I came up with some shark attack nails ? 😭😭</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgiw02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1lggma7</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>What to do? Cured gel over cut</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lggma7/what_to_do_cured_gel_over_cut/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1lgi162</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>What do yall think so far</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hr7ck7j068f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1lgi8jw</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>I can’t believe I waited 25 years to start getting my nails done- never going back!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ct5bw40c268f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1lgi3iw</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>🍃💚</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgi3iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1lghicg</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>🫐🍓</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lghicg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1lggzrm</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>I'm just so obsessed!!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lkzhbod1s58f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1lggz0w</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>I always hate my nails. I want coffin, I get that they’re too short for that, but they’re always too thick and look bad. So every time I go to a different place. I live in a very rural area, so my options are limited. Most recently, she convinced me to try builder gel. This is the result.</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lggz0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1lggqlu</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Getting better at these press ons</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p13tvc21q58f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1lgd4pq</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>"It's never enough, love"</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgd4pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1lge867</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Are my nails damaged?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lge867</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1lgektp</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>just found this forum so my nails are already a bit outgrown! but i love to show them off, i love them!</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qs4hg2e958f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1lgf3d1</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Are they really bad?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgf3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1lgf4rt</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Press-on sizing</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/neggkz6jd58f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1lgf1fx</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Nail Envy Ruined my nails</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/804sfs0uc58f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1lgex2p</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Cute press on that I made instead of studying lol!!!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgex2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1lgenyf</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>summer nails</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mzatdz1a58f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1lgenq2</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Gay frog nails 2.0 - acrylics + builder gel, done by @naildbyveronica</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgenq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1lgem0y</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>My nails for a concert.</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rftknnmn958f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1lgeiyk</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>I needed Goddess nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lnr5lfz858f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1lgefmd</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Mermaid pearl nails to match my dress 🧜🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgefmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1lgef5u</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>cute frog nails!!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83cwrp45858f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1lgeel0</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>First time in a long time</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/509m1s32858f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1lge6iw</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Summer white and pink</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o36lj1vc658f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1lgdy2c</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Did French for the 1st time in my life. A colourful one because I hate it classic</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4ch3m6l458f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1lgdtr2</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Adhesive tape or nail glue?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgdtr2/adhesive_tape_or_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1lgdmyl</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My natural nails after years of being a chronic nail biter</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgdmyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1lgdfyt</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>First time getting acrylics!!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgdfyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1lgddxp</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>My nail artist is amazing! Hand painted 😍</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgddxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1lgd6ng</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Feeling fishy 🎣</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twbm0pvuy48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1lgcygh</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>I did nails for my friend as a beginner 💖</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgcygh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1lgcwv6</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Pearl Frenchies!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pc3n26mrw48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1lgc5tz</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bgrpuk4r48f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1lgbb0p</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>These glue ons from target are amazing</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgbb0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1lgark8</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>My gelx nail came of with my nail, it’s my grad tn!</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgark8/my_gelx_nail_came_of_with_my_nail_its_my_grad_tn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1lgbq7l</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>miffy nails~</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgbq7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1lgbmzu</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Can these nail pages be trusted?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgbmzu/can_these_nail_pages_be_trusted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1lgbdur</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>looking for general nail advice 😭</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgbdur/looking_for_general_nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1lgb3v8</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Wild cherry nails 🍒</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgb3v8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1lgarmr</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Rhinestone nails</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znvcyz80h48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1lga4ul</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>My gelx nail ripped off along with my natural nail. It’s my graduation tonight and I’m freaking out</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7qlecdec48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1lgakhs</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Why do my nails curve down as they grow?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgakhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1lg9y3g</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>4th of July press on nail set I made as a nail tech with tourrettes syndrome</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3x05ry34b48f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1lg9zos</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Did my nails myself :) love press ons</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg9zos</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1lg9uwy</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>I LOVE THI SET</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysr48g7ga48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1lg9k9h</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Spooky</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2gpuh9d848f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1lg9edp</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Just got home from salon and nails have just started looking like this m?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/130snlf6748f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1lg9ewx</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Gold &amp; Black 💛🖤</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wzdzb9a748f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1lg9792</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Are these acrylics as bad as I think</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg9792</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1lg9c93</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Ducky nails 💅</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4yuinar648f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1lg9asl</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>My own nails with shellac I can’t believe how great they look ❤️🥰</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ggvj65h648f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1lg97fq</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Blue Bday nails</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg97fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1lfq1jb</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>How can I fix my nails?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cinkwrp84z7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1lg0kik</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Starting my DIY nail journey!!</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lg0kik/starting_my_diy_nail_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1lg5hsk</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>How to choose an at home nail tech?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lg5hsk/how_to_choose_an_at_home_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1lg8r9s</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>New Nails for Summer 🐚🌊</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg8r9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1lg8rx9</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Pride Butterflies with matching makeup</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0phk9hfp248f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1lg6c2d</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>I need help! I want to switch over to gel-x. I don’t know if I should just natural or sculpted..</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg6c2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1lg8xh0</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>New Summer Nails ✨I just wish I could stop biting off my skin around them 😅</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zihdv95u348f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1lg8kop</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>How to prevent nail from warping(?)</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg8kop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1lg8hvg</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>$142 Nails from yesterday</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg8hvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1lg8bwn</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Cute little vintagey set I did yesterday</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg8bwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1lg82m3</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>I like these pics sm better lol but still so obsessed with these nails</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg82m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1lg5t4h</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>did i get lied too?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg5t4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1lgra0k</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>A good base coat and glass file goes a long way 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgra0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1lgl22w</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>New to nail care after quitting hard gel - how can I get started?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0pxwgior68f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1lgny68</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>First attempt at magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwizque1k78f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1lgqrex</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Help me find this color</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib4w77yhf88f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1lgp8gd</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Fruity Portraits and my Pride Flag! 🍒🍊🫐🍓🍐🏳️‍🌈🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgp8gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1lgp5o3</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>You know her, you love her 🍄</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e5zbupi0x78f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1lgp36f</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>💚 Emerald City &amp; The Price is Alexandrite 💜</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0f33xmc9w78f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1lgo7dg</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Favorite flakies?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgo7dg/favorite_flakies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1lgnt9i</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>ISO indie brands with fast shipping [WA, USA]</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgnt9i/iso_indie_brands_with_fast_shipping_wa_usa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1lgnli9</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>I’m not doing great and neither are my nails</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgnli9/im_not_doing_great_and_neither_are_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1lgmws4</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>An HHC &amp; PPU summer mani</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30bto0qd978f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1lgmqf8</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Look what I found!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgmqf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1lgmlpy</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>I Love/Hate Essie’s Bodice Goddess</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgmlpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1lgl0h5</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>New hyperfixation</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b4dehkm8r68f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1lgks80</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Dazzle Dry's weird marketing</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbudz5ruo68f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1lgkfb8</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Help! I nailed it, then un-nailed it, with magnetic mani🙏</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9w0bmqbql68f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1lgk7r3</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Too Hot to handle</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgk7r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1lgk7g7</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Organization bliss</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgk7g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1lgjsw4</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Finally long enough for ~a shape~</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci1mt04if68f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1lgjeki</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Dr. Pepper stans rise up 🫡</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgjeki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1lgijsg</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Anyone have real swatch pics of Lurid - Stargazing On Solstice and As the Long Dark Night Gives Way to Morning</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgijsg/anyone_have_real_swatch_pics_of_lurid_stargazing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1lgiiv7</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Day 1 Of Asking Your Opinion On A Polish Brand: Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgiiv7/day_1_of_asking_your_opinion_on_a_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1lgie7o</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Rock candy 🍬</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgie7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1lgi8js</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Cracked Polish's The Shag is so beautifully sophisticated 💚</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgi8js</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1lgi8an</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Dupe for Hermès Iris Violetta - or your favourite creamy lilac/purple shade?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgi8an</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1lgi7fz</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>BKL Drop-Sold Outs</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgi7fz/bkl_dropsold_outs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1lgi5rn</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Mass Wisteria! Anniversary polish celebrating the Reddit Lacquerist Discord 💜🤍💙 [Paid PR]</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/opzi876o168f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1lgi5rr</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>BKL Undoing vs Mooncat Ribbit</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgi5rr/bkl_undoing_vs_mooncat_ribbit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1lghokr</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Chamaeleon - Strawberry Dartfrog</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lghokr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1lghm2k</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>10 free French tip base recommendations?</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lghm2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1lgha6e</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Subtle pride nails!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns4q4dxdu58f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1lgh9es</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Can't-miss polishes from Lurid Lacquer?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgh9es/cantmiss_polishes_from_lurid_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1lgh1du</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Accidentally matching!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aymlwdjfs58f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1lgguiy</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/onm21x5rq58f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1lgfzt6</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>My first shimmer💛</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgfzt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1lgfm2u</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>💛 Painted Polish Fury &amp; Fantasy 🤍</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1jir5k7h58f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1lgfhxu</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Neon Tropical Summer</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgej2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1lgfeja</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>❤🧡💛💚💙💜</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgfeja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1lgfdu5</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>When a post says "Skittles" what does that mean?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgfdu5/when_a_post_says_skittles_what_does_that_mean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1lgev9p</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>I can’t stop staring at my nails 🤩</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/boyz67rjb58f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1lgecnv</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Looking for Colors in a Certain Palette</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o65epgpn758f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1lgeb8y</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Magnetics are worth the wait. 🌠</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgeb8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1lge05p</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>BKL Question</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lge05p/bkl_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1lgdsx3</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Blood orange polishes similar to MC Pandemonium?</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gaha5fi358f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1lgdns6</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Bubble Mew 🩵</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgdns6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1lgd7s7</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Best BKL polishes?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgd7s7/best_bkl_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1lgckf5</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>How do you fly with nail polish?</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgckf5/how_do_you_fly_with_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1lgbsck</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Revisiting my older magnetics now that I’ve got this technique down!</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/su60196ho48f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1lgbe57</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Looking for the juiciest, glossiest toluene free top coat</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgbe57/looking_for_the_juiciest_glossiest_toluene_free/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1lgb9pd</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Tired of professionally lit swatches being the main showcase</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgb9pd/tired_of_professionally_lit_swatches_being_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1lgavx9</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Devastating delivery</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21epd1luh48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1lgaut5</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Dollar Tree Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kfgipsmh48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1lgaok4</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Trying some thrifted nail polish. 50c each sounded like a no-brainer to me.</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgaok4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1lgag69</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>I can't believe how pretty Flower Child is🌺✨️</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgag69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1lg9mkc</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Dazzle dry comparisons</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l4cyrvs848f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1lg9hzj</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Weird discoloration after gel manicure? Doesn't hurt or anything, having the gel on didn't hurt or itch or anything neither</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzbw0mzw748f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1lg9ck3</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>My first ILNP - Fairy Dust ✨🧚‍♂️</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg9ck3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1lg90vj</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>This might be my new favorite red ❤️</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qms9atpi448f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1lg8h5y</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Watermelon Sherbet🍉</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg8h5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1lg8cx2</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>my mother’s hands</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cweicoqmz38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1lg8a96</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>I already have a lifetime supply of polish</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>/r/AskReddit/comments/1lfszbs/you_just_won_a_lifetime_supply_of_the_last_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1lg7jnl</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Spring fairy feels 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofc7nf3ut38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1lg7dcv</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Neon Dreams collection from Aura Bloom Polish (small indie brand!)</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg7dcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1lg77bf</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>How to do “pool nails” with regular non gel polish</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx1v71odr38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1lg74ik</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Doing gel after contact dermatitis</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lg74ik/doing_gel_after_contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1lg6w4r</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>This may be the last hurrah for my very old bottle of Essie's Shine of the Times</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vj995nvo38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1lg6nq0</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>ILNP Blue Print</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg6nq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1lg6i6l</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Summer is for neons!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg6i6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1lg6fdy</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Heading to Santa Rosa Beach today! ☀️</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg6fdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1lg68q5</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Help identifying this polish 🙏</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl8l8srhk38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1lg5iub</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>🌙 moon jelly 👻</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i6kvpx7f38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1lg5ckt</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Favorite Base and Top Coat?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lg5ckt/favorite_base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1lg5aga</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Ummm new favorite</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xz9z56hd38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1lg52qs</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Hot Damn 🥵</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg52qs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1lg4yxr</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Help me identify this color?!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg4yxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1lg4tt3</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Cracked order 💜</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1y9ixiyy938f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1lg4o8a</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈🩷🤍Genderfluid Pride Flag🖤💜🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg4o8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1lg4bdk</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Summer’s no reason to stop  giving off witchy vibes 🪄✨</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg4bdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1lg2eya</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Chrome powder first timer</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8la3jppp28f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1lg11s1</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>In my soft girl summer era</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg11s1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1lg0xs1</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Flash on ⛈️</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg0xs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1lg0f8f</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Sheer natural nail polish</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lg0f8f/sheer_natural_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1lfzbzg</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Vaporwave &amp; Summer by ILNP</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lfzbzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1lfz372</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Experience Packing Polish for a Move?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l9ct8ojp18f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1lgqguo</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>A very delicate almond that seems like the first time 🥹🫣</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgqguo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1lgq7kv</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Lisa Frank nails for summer</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgq7kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1lgpxcu</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>aquarium nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jw3kz4q588f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1lgpbqv</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Mermaid nails 🧜🏻‍♀️✨💙</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgpbqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1lgoon3</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Stitch Nails 💙</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgoon3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1lgligc</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Swipe for the inspo ➡️✨💜</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgligc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1lgfxu6</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Whatchyall Think ... Nail Set By Me Off Course 😌🤏🏿✨️</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgfxu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1lgdlfe</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>what design do i get on my thumbs?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kme3fetz158f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1lgcv7l</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>my nails</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2bjyjuew48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1lgcuj7</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>How to bend these metal charms</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgcuj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1lgcdjy</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>First character set 🍒⛓️</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgcdjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1lgc7va</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>First design, how can I improve? ✨</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ix1nqh5kr48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1lgawk3</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Love how good these turned out!</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83njk7fxh48f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1lg7fiq</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>My tech just turned 20 &amp; is so talented she’s def going far she kills it every time!</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39n79s50t38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1lg6wrj</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>First time trying tape to make lines.</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg6wrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1lg5v9x</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>I don't know if I'm in the right world 😫</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gze4oyash38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1lg54a3</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Made by me 🧚🏼‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p07th9s6c38f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1lg1brf</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>I finished the fairy core press on nail set!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lg1brf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1lg1906</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>EU people!! Where do you buy nail art deco and figures?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lg1906/eu_people_where_do_you_buy_nail_art_deco_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1lfzti9</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>I drew some bright colored flowers on my nails !</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbl34k9ay18f1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun 22 08:11:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_22.xlsx
+++ b/data/collected_data/2025_06_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1287"/>
+  <dimension ref="A1:C1481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22312,6 +22312,3304 @@
         </is>
       </c>
     </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1lhin22</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Does this color look bad on my skin??</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6deebdg1rf8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1lhhdip</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>I love how the decoration of this set turned out! When you learn to use chrome powder you can do many beautiful things 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/diua8thwbf8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1lhhbq7</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>New nails!!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06skexnbbf8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1lhh3t1</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>My favourite set yet</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7plcvaxq8f8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1lhgv2k</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>SERIOUSLY NEED HELP !</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elfsbxp06f8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1lhg3w3</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Fresh Set For The Summer ❤️</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhg3w3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1lhfv5w</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Accidently got spunk colored nails. Woops</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9eog090vue8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1lhfoxf</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>✨🌺</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sgmvk9xse8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1lhfove</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Are my nails supposed to be bendy???</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lhfove/are_my_nails_supposed_to_be_bendy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1lhevh7</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Looking for gel dupe of Essie polish</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9pdyvd4ke8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1lhesqj</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Obsessed with cat eye polish😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6l4a7klcje8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1lheo9h</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Natural nail overlay transformation! Content warning for damaged nails 😵</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lheo9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1lhe7yb</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Sad Nails</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhe7yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1lhe7qi</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>I love my nail tech !</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/127inpv8de8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1lhdyjk</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Loving this milky white glitter!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhdyjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1lhdn1y</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Beetle gel nails at home tips</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lhdn1y/beetle_gel_nails_at_home_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1lhdjfl</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Manicure natural nails with rubber base, I love that they look natural and simple</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhdjfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1lhdipq</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Summer melon</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwwm717d6e8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1lhd9t1</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>No one mentioned Russian manicures are addicting</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly6diphx3e8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1lhd2qp</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Pride nails 🏳️‍🌈✨✨</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhd2qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1lhcilt</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Rainbow Skittle with Thermal Polishes 💖</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhcilt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1lhcgwz</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Fourth July set.</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi8kugzyvd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1lhcfhl</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Nude pink with a feature nail</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytfhh2alvd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1lhca0n</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>I painted my nails:3</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yo9jv2e2ud8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1lhc5p2</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>After 6 years, I'm finally satisfied with my work, but there's always room for improvement!</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0jqb66tsd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1lhbqyl</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Ceramic tile nails! They look so much better in person</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhbqyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1lhbioy</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Basically build-a-bear 😭</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhbioy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1lhbih4</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>How do they look?</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnx57u5smd8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1lhbg4z</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Made these for a friend ♥️</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyllzrg6md8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1lhbfpp</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Some green maybe?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smo3a3m2md8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1lhbbrg</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>My nail tech never fails to give me life</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhbbrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1lhb9fy</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Toenail (gel)polish won’t stay on??</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lhb9fy/toenail_gelpolish_wont_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1lhb8z7</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>My nail has seen stuff</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0u23nrakd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1lhahg9</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>4th/beachy vibes</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qhgrcqddd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1lhaf1j</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Looks like I just went to the salon?</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhaf1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1lha7iv</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Sharing nails I’ve had :)</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lha7iv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1lh9zjq</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>my summer mani!</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh9zjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1lh9rft</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Game Day means Nail Day. Happy Soltice, Summer, and Pride everyone!</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh9rft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1lh9qfq</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Why does it feel wrong?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh9qfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1lh9ls5</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Switched from dip to builder gel</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebcxhfgk5d8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1lh867b</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>My best work yet</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh867b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1lh7182</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>First time 3-d Gel Flowers (two styles)!</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh7182</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1lh9c10</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Fishy nail art</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh9c10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1lh985j</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Got my nails done for my birthday 🎂</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnnff9t92d8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1lh8z72</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>New nails. What should these have cost?</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5104w8i30d8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1lh8jbi</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>My nail broke 😭</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsdlh9lbwc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1lh80zk</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Gel-X 🎱🍒</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh80zk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1lh7vhv</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Finally</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hfcysjjnqc8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1lh7ud7</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Summer vibes 🐚🩷</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26jce6c9qc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1lh7u7t</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>I did these yesterday, I'm new to doing my nails so they took hours lol ♡</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqa2o42dqc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1lh7m73</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>pride nails!</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn2kg91goc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1lh7cuk</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Hand painted 🥰</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptx07kdcmc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1lh72aj</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>I've been experimenting with some new nail art styles recently &amp; I LOVE creating designs like this!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh72aj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1lh6zu9</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Nail Idea</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36jrp0ucjc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1lh6zl5</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Red nails never disappoint</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuwo28pajc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1lgrijg</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Melodysusie P-Plus20F lamp - do you like it?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgrijg/melodysusie_pplus20f_lamp_do_you_like_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1lgs538</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>I’m lost on what to do with this nail what has happened to it</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgs538</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1lguu4r</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Why do I have never ending cuticles</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lguu4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1lgx5um</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Nails lifting help, noob advice please</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lgx5um/nails_lifting_help_noob_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1lgxrit</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgxrit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1lh6utl</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>pride nails!</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3uu4ez14ic8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1lh6mno</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Another option</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd3vuoscgc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1lgyxxw</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>DND Gel Shade Match</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x12dgxqwra8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1lgwttn</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Mermaid Inspo</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u82jx0amaa8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1lgv6jf</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>It wasn't what I wanted, they looked very strange! I don't know why they look bad, what's weird???</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atbrpzuhv98f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1lgvccf</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>My partners gel French tip Moroccan summer inspired nails. With little hand painted lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz563yu3x98f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1lgxvwj</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>gel x lifting after 1 week</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgxvwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1lgyj1z</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Nails I did yesterday</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28ehhb9ooa8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1lh5eun</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Can’t Get These Press-Ons Off! Please Help 😭</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx95n2re6c8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1lh1xa5</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Do techs normally cut their clients' cuticles?</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh1xa5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1lh3au9</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Regular Nail Polish Just Won’t Dry</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lh3au9/regular_nail_polish_just_wont_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1lh659x</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>I think these are the cutest!!</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n90jsvdcc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1lgu47f</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Which length is best?</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgu47f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1lgtejm</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>cracked the polish but not the nail?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cq3qvq56c98f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1lgr2b5</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Help finding nail design</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/590skt07j88f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1lh5wex</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Trust the process 🤣</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh5wex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1lh5ssk</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>What do y'all think?</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggqurb7i9c8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1lh5kvg</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Birthday nails 💙</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abb02jgq7c8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1lh5fqy</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Nail growth after one week smh no</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh5fqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1lh4hny</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Fruit nails!</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kphjxz9zyb8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1lh4dfw</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Lazy girl diy nails</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lh4dfw/lazy_girl_diy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1lh464h</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Custom press on set! 🖤⚜️</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh464h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1lh3tar</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Pokemon Gold vs Silver</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh3tar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1lh3iya</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Looking for a non-leveling fluffy gel</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/un52lvjhrb8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1lh33we</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>time for a fill in under 2 weeks?</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syytus75ob8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1lh2xlw</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Nails for vacation💎</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh2xlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1lh2w1z</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Engagement Nails 💐</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh2w1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1lh2tj6</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>The sunlight is hitting my new manicure so beautifully</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdbahugslb8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1lh2kp2</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>First time trying press-ons for toes</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0ta52g1kb8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1lh26x4</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>I’ve never seen this method before, good idea of not?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh26x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1lh25rc</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Summer holiday nails~</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2t81i6xgb8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1lh1w4a</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>DIY gel manicure, super happy with this set</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh1w4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1lh1mb7</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Gothic Starlight nails :3</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ul5cmoyocb8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1lh18xm</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Are they cute?</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh18xm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1lh0q3z</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/su489uev5b8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1lh0jb6</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Hand Drawings</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qiv120e4b8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1lh07n9</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>New nails i loveee them</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzh868mu1b8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1lh03en</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>New nails! Gone short this time, need to gain some strength again! 💜</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5a1eupx0b8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1lgzn36</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>For all the purple girlies</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgzn36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1lgzawe</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>~Waves + French~</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dims59upua8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1lhi8r4</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Pastel Pride Nails</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhi8r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1lhhea0</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Did Only One Bed come back and not get announced in the overpours?</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9513mzc5cf8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1lhh0uc</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>My first Lurid Lacquer order!</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtct41vs7f8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1lhfpw3</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Ghost Ship⛵️</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bry2l9t7te8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1lhfg8z</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Velvetizing with $1 magnet I found at the local dollar store</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sn3ofzh1qe8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1lhffl7</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Bisley is doing a summer sale right now</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/us9q8b21qe8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1lhfduc</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Cirque Colors fans I have a Q</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhfduc/cirque_colors_fans_i_have_a_q/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1lhfb2o</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Some collabs I have</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhfb2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1lhf8ig</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Do you use rubbing alcohol or acetone to dehydrate your nails?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhf8ig/do_you_use_rubbing_alcohol_or_acetone_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1lhf79s</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Look what I Found update pt 2</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhf79s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1lhf46f</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>First time using charms ✨️</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhf46f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1lhemtt</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Finally found it! Update pt 1</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhemtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1lhedoh</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Creams?</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhedoh/creams/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1lhdkvm</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>A brand with a full rainbow linear holo collection?</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhdkvm/a_brand_with_a_full_rainbow_linear_holo_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1lhdc8s</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Red Hot ♥️</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhdc8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1lhd45h</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Very sheer pink glittery nails with Canmake polishes</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7iopo6371e8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1lhczl7</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Another fake Starrily website</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhczl7/another_fake_starrily_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1lhcq9q</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Fairy nails experiment</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oqth6t5hyd8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1lhcn1v</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>First jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhcn1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1lhck6i</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>I'm in heaven</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/765to16wwd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1lhca3y</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Wild Magnetic!</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ikrcrnv3ud8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1lhc1pf</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Pearly white 🫧</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhc1pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1lhbxq4</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>What is the greenest green?</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhbxq4/what_is_the_greenest_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1lhbviy</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Mooncat brought me here, but I'm staying for BKL.</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhbviy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1lhbhj1</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Nail peeling mystery culprit?</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhbhj1/nail_peeling_mystery_culprit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1lhaytq</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Forever Repurchase: Black</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhaytq/forever_repurchase_black/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1lham70</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>My Very First Knockwurst powder dupe?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/at6coihjed8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1lhajky</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Matchy matchy!</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5noiaaawdd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1lhaiq5</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Day 2 of asking your opinion on a polish brand: LA Colors</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lhaiq5/day_2_of_asking_your_opinion_on_a_polish_brand_la/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1lh9ixg</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Rainbow on my fingers</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh9ixg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1lh8z27</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Nailtiques 2 users</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lh8z27/nailtiques_2_users/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1lh8w9k</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Jade Drake from Arcana Lacquer</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh8w9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1lh7sw2</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Every week I change my nails to one of my boyfriends interests while he’s away for work</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6qi0cp1qc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1lh7ptj</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Pink and Purple Flakie Polishes</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lh7ptj/pink_and_purple_flakie_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1lh7m32</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Convince me to buy your #1 favorite polish of all time</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lh7m32/convince_me_to_buy_your_1_favorite_polish_of_all/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1lh7i6d</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>What brands make the best Glow in the dark, Blacklight UV light whatever nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lh7i6d/what_brands_make_the_best_glow_in_the_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1lh752g</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>the brightest polish I own so far</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh752g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1lh74ry</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>ILNP - Tidal Wave</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh74ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1lh73l5</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>My florals look like my flesh 🙃😌</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ohfnnv6kc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1lh71pi</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Hard gel + See through + Iridescent top coat</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/542li8vrjc8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1lh70z4</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>A very bad attempt at a very 2013 ace pride nail set</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh70z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1lh6yyg</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>trans pride mani 🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh6yyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1lh65xl</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>What's our 90%?</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7m2neejcc8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1lh649t</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Anyone else loathe beautiful sheer polishes?</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lh649t/anyone_else_loathe_beautiful_sheer_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1lh5ppr</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Nail polish gets darker after application</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lh5ppr/nail_polish_gets_darker_after_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1lh4u2j</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Polished for Days Gleam</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/azadhlhs1c8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1lh4n4m</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Spotted Cupcake in the wild</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ju9j5d870c8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1lh4h1b</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>How to?</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6tsccrtyb8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1lh3mq9</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>🦎Lizard Toe Hairs🦎</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh3mq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1lh3gbz</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Sundown🌅</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh3gbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1lh3dp0</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Cirque Colors Strawberry Fields</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh3dp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1lh3bwd</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Polish like this?</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh3bwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1lh34ow</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>You already know the polish name.</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/migeyep9ob8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1lh1il2</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Non-thermal dupe for Treachery in the Blue (in the cold state)?</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpmkyarwbb8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1lh1dd4</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>first time purchasing not drugstore polish</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0285ijstab8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1lh134a</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Soft dusk sky</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh134a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1lh0ubd</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Love seeing how this polish changes in different lighting!</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh0ubd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1lh0c03</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Color to match my outfit?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv79rs6s2b8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1lh05vh</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Pan flag for Pride, first time gradient 🫣</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh05vh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1lh02f2</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Pride 2025 Nails</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32vrllgn0b8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1lgzryx</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Scared of my allergy</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgzryx/scared_of_my_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1lgz8v3</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>How do you get the shine bac</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgz8v3/how_do_you_get_the_shine_bac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1lgz5r9</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>DND Gel Shade Match</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlu0te1nta8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1lgyyrc</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>A true pink shimmer topper without shift?</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgyyrc/a_true_pink_shimmer_topper_without_shift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1lgywoh</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Bless Your Heart by Holo Taco 💖</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypcoccv0qa8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1lgysu1</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Dark and Twisted Lacquer's Gothic Fairy (LBOH)</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgysu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1lgrwxf</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Tried Layering + Recs?</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgrwxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1lgyhxu</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>colored jelly magnetics vs translucent magnetic and pairing with jelly polish</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgyhxu/colored_jelly_magnetics_vs_translucent_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1lgyg0p</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Funny Business Let's Take This Offline</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7hqfy5zna8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1lgy123</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Bless your heart 💕</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvzl4h7kka8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1lgxpwv</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Matched my nails to my son's dinosaur toy!</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xep38c3yha8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1lgxc6i</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>BKL Not Tonight</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgxc6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1lgx6t7</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Pride skelly bois 🌈💀</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhgglphqda8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1lgw6wt</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Did myself some nail art for pride 🌈✨</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgw6wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1lgu3aj</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>What are your favorite glitter polishes?</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lgu3aj/what_are_your_favorite_glitter_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1lhgizi</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>My nails the last few months!</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhgizi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1lhgbj5</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Monet inspired nails</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhgbj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1lhdagy</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>This week’s set</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhdagy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1lhd9vh</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Wanted some summer nails</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1t7xexx3e8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1lhckx1</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>My sister did my nails with soot sprites from Totoro</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lhckx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1lhcdde</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Fresh ombré</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwsqi550vd8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1lh71bq</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Chrome press on set! 🖤⚜️</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh71bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1lh5d6y</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Simple, but beautiful and subtle</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zv2pud926c8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1lh53qk</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>lion king nails :)</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh53qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1lh3tpf</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh3tpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1lh1b63</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh1b63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1lh197y</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lh197y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1lgzhsp</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Pokemon Gold vs Silver</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgzhsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1lgzgbx</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Just having fun</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgzgbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1lgxnp2</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>I made a video of my nail art.</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cu7xew1hha8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1lgw5a4</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>My Pride Mani 🌈✨</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgw5a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1lgv83a</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Obsessed with these nails I did</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgv83a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1lgufri</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Did this Alice in wonderland themed set (for free) for a friend, any tips on how to improve ?</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lgufri</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1lgucop</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Detailed Hand-Painted Gothic Bugs on these Coffin Nails! ✨</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pz1ckwwm98f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>